<commit_message>
🔄 Actualización automática del mapa (2025-10-08 08:24:16)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Traspasos.xlsx
+++ b/mapa_interactivo_Traspasos.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -870,27 +870,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3659</t>
+          <t>3765</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/2/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ALBERTI 59</t>
+          <t>NAZCA AV. 1675</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>797489950</t>
+          <t>798295165</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso y Retiro PROPIO</t>
+          <t>Columna con base picada</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -913,12 +913,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -927,24 +927,24 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.401798</v>
+        <v>-58.47874</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.61024</v>
+        <v>-34.61462</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -956,27 +956,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>3830</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>NAZCA AV. 1675</t>
+          <t>COLOMBRES 75</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>798295165</t>
+          <t>798385574</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Columna con base picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1013,24 +1013,24 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.47874</v>
+        <v>-58.419354</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.61462</v>
+        <v>-34.612362</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1042,7 +1042,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3830</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1052,17 +1052,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>COLOMBRES 75</t>
+          <t>Rincon 343</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>798385574</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1093,16 +1093,12 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>-58.419354</v>
+        <v>-58.396196</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.612362</v>
+        <v>-34.613511</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1116,7 +1112,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>CEN-C</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1128,32 +1124,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Rincon 343</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1163,7 +1159,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1176,19 +1172,19 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
-        <v>-58.396196</v>
+        <v>-58.395656</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.613511</v>
+        <v>-34.590364</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1198,7 +1194,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-C</t>
+          <t>RET-C</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1210,32 +1206,32 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1245,7 +1241,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1258,29 +1254,33 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr"/>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M10" t="n">
-        <v>-58.395656</v>
+        <v>-58.458354</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.590364</v>
+        <v>-34.564883</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>RET-C</t>
+          <t>COG-G</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1292,17 +1292,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>-143</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>10/7/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1312,12 +1312,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>797752816</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1325,13 +1325,9 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Base picada</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1349,14 +1345,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.458354</v>
+        <v>-58.458864</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.564883</v>
+        <v>-34.561167</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1366,7 +1362,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>COG-G</t>
+          <t>COG-H</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1378,17 +1374,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-143</t>
+          <t>5589</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10/7/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
+          <t>ARCOS 1520</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1398,12 +1394,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>797752816</t>
+          <t>799540526</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1411,7 +1407,11 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
@@ -1431,14 +1431,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.458864</v>
+        <v>-58.449125</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.561167</v>
+        <v>-34.565958</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>BLO-M</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1460,32 +1460,32 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>5589</t>
+          <t>4082</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>12/21/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ARCOS 1520</t>
+          <t>MERCEDES 254</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>799540526</t>
+          <t>801901755</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1495,11 +1495,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R200 para pedir traspaso de equipo</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1517,14 +1517,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.449125</v>
+        <v>-58.484232</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.565958</v>
+        <v>-34.631431</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1534,44 +1534,44 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-M</t>
+          <t>DEV-L</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4082</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>12/21/2024</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MERCEDES 254</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>801901755</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Colocar R200 para pedir traspaso de equipo</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1599,65 +1599,65 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.484232</v>
+        <v>-58.397512</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.631431</v>
+        <v>-34.609923</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>DEV-L</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1685,28 +1685,28 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.397512</v>
+        <v>-58.496935</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.609923</v>
+        <v>-34.599084</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>PUE-B</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1718,32 +1718,32 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>4862</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>ARCOS 2263</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>802857379</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1753,11 +1753,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1775,14 +1775,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.496935</v>
+        <v>-58.455082</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.599084</v>
+        <v>-34.558883</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>PUE-B</t>
+          <t>BLO-P</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1804,32 +1804,32 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4862</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ARCOS 2263</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>802857379</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1837,11 +1837,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>picada</t>
-        </is>
-      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
         <v>0</v>
       </c>
@@ -1852,23 +1848,23 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.455082</v>
+        <v>-58.487666</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.558883</v>
+        <v>-34.649704</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1878,7 +1874,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>BLO-P</t>
+          <t>PAV-N</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1890,32 +1886,32 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1923,9 +1919,13 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+        </is>
+      </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1934,33 +1934,33 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.487666</v>
+        <v>-58.441405</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.649704</v>
+        <v>-34.594348</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>PAV-N</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1972,7 +1972,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1982,17 +1982,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2005,11 +2005,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
-        </is>
-      </c>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
         <v>1</v>
       </c>
@@ -2029,14 +2025,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.441405</v>
+        <v>-58.483821</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.594348</v>
+        <v>-34.677698</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2046,7 +2042,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>PAV-Q</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2058,32 +2054,32 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2091,7 +2087,11 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I20" t="n">
         <v>1</v>
       </c>
@@ -2107,18 +2107,18 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.483821</v>
+        <v>-58.404913</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.677698</v>
+        <v>-34.615857</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>PAV-Q</t>
+          <t>CEN-M</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2160,7 +2160,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2188,23 +2188,23 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.404913</v>
+        <v>-58.394304</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.615857</v>
+        <v>-34.621645</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>CEN-M</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2226,27 +2226,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2283,10 +2283,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.394304</v>
+        <v>-58.391419</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.621645</v>
+        <v>-34.605543</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>CEN-E</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2312,7 +2312,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2322,17 +2322,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2347,7 +2347,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2360,7 +2360,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2369,14 +2369,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.391419</v>
+        <v>-58.394118</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.605543</v>
+        <v>-34.601416</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CEN-E</t>
+          <t>RET-H</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2398,32 +2398,32 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2455,24 +2455,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.394118</v>
+        <v>-58.451835</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.601416</v>
+        <v>-34.562646</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>RET-H</t>
+          <t>BLO-N</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2484,32 +2484,32 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2519,11 +2519,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2541,24 +2541,24 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.451835</v>
+        <v>-58.406585</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.562646</v>
+        <v>-34.592933</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>BLO-N</t>
+          <t>AGU-B</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2570,32 +2570,32 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2605,11 +2605,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2618,7 +2618,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2627,14 +2627,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.406585</v>
+        <v>-58.401624</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.592933</v>
+        <v>-34.612001</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2644,7 +2644,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>AGU-B</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2656,17 +2656,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>ICD31456940</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2689,11 +2689,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
-        </is>
-      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
         <v>1</v>
       </c>
@@ -2704,7 +2700,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2713,10 +2709,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.401624</v>
+        <v>-58.400169</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.612001</v>
+        <v>-34.617784</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2730,7 +2726,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>CEN-N</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2910,27 +2906,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2945,7 +2941,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2963,18 +2959,18 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.413584</v>
+        <v>-58.435017</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.58551</v>
+        <v>-34.622044</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2984,7 +2980,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>AGU-L</t>
+          <t>PCH-M</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -2996,17 +2992,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3016,7 +3012,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3031,7 +3027,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3044,7 +3040,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -3053,10 +3049,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.435017</v>
+        <v>-58.443232</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.622044</v>
+        <v>-34.620007</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3070,7 +3066,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PCH-M</t>
+          <t>PCH-G</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3082,32 +3078,32 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7229</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AZURDUY JUANA 2627</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>ICD30814490</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -3117,7 +3113,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Colocar columna para pedir traspaso de nodo propio</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3135,117 +3131,31 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.443232</v>
+        <v>-58.469008</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.620007</v>
+        <v>-34.552083</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>PCH-G</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>7229</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>9/16/2025</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>AZURDUY JUANA 2627</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>ICD30814490</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Colocar columna para pedir traspaso de nodo propio</t>
-        </is>
-      </c>
-      <c r="I33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M33" t="n">
-        <v>-58.469008</v>
-      </c>
-      <c r="N33" t="n">
-        <v>-34.552083</v>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>COG-L</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>
@@ -3262,7 +3172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3529,27 +3439,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3659</t>
+          <t>3765</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10/2/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ALBERTI 59</t>
+          <t>NAZCA AV. 1675</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>797489950</t>
+          <t>798295165</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3564,7 +3474,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso y Retiro PROPIO</t>
+          <t>Columna con base picada</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -3572,12 +3482,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -3586,24 +3496,24 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.401798</v>
+        <v>-58.47874</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.61024</v>
+        <v>-34.61462</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -3615,27 +3525,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>3830</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NAZCA AV. 1675</t>
+          <t>COLOMBRES 75</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>798295165</t>
+          <t>798385574</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3650,7 +3560,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Columna con base picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -3663,7 +3573,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -3672,24 +3582,24 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.47874</v>
+        <v>-58.419354</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.61462</v>
+        <v>-34.612362</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -3701,7 +3611,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3830</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3711,17 +3621,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>COLOMBRES 75</t>
+          <t>Rincon 343</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>798385574</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -3736,7 +3646,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -3752,16 +3662,12 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>-58.419354</v>
+        <v>-58.396196</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.612362</v>
+        <v>-34.613511</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -3775,7 +3681,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>CEN-C</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -3787,27 +3693,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Rincon 343</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -3822,7 +3728,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -3838,26 +3744,30 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M7" t="n">
-        <v>-58.396196</v>
+        <v>-58.458354</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.613511</v>
+        <v>-34.564883</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>CEN-C</t>
+          <t>COG-G</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -3869,27 +3779,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -3904,7 +3814,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -3922,28 +3832,28 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.458354</v>
+        <v>-58.397512</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.564883</v>
+        <v>-34.609923</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>COG-G</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -3955,27 +3865,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -3988,13 +3898,9 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>PIcada</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -4003,7 +3909,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -4012,24 +3918,24 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.397512</v>
+        <v>-58.487666</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.609923</v>
+        <v>-34.649704</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>PAV-N</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -4041,27 +3947,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -4074,9 +3980,13 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -4085,7 +3995,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -4094,24 +4004,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.487666</v>
+        <v>-58.404913</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.649704</v>
+        <v>-34.615857</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>PAV-N</t>
+          <t>CEN-M</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -4123,7 +4033,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4133,7 +4043,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -4143,7 +4053,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -4158,7 +4068,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -4171,23 +4081,23 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.404913</v>
+        <v>-58.394304</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.615857</v>
+        <v>-34.621645</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -4197,7 +4107,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-M</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -4209,27 +4119,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -4244,7 +4154,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -4257,7 +4167,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -4266,10 +4176,10 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.394304</v>
+        <v>-58.391419</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.621645</v>
+        <v>-34.605543</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -4283,7 +4193,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>CEN-E</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -4295,7 +4205,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -4305,17 +4215,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -4330,7 +4240,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -4343,7 +4253,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -4352,14 +4262,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.391419</v>
+        <v>-58.394118</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.605543</v>
+        <v>-34.601416</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -4369,7 +4279,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>CEN-E</t>
+          <t>RET-H</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -4381,17 +4291,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -4401,7 +4311,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -4416,7 +4326,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -4429,7 +4339,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -4438,10 +4348,10 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.394118</v>
+        <v>-58.401624</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.601416</v>
+        <v>-34.612001</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -4455,7 +4365,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>RET-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -4467,17 +4377,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -4487,7 +4397,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>ICD31456940</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -4500,11 +4410,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
         <v>1</v>
       </c>
@@ -4515,7 +4421,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -4524,10 +4430,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.401624</v>
+        <v>-58.400169</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.612001</v>
+        <v>-34.617784</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -4541,7 +4447,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>CEN-N</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -4553,27 +4459,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4588,7 +4494,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -4606,18 +4512,18 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.413584</v>
+        <v>-58.435017</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.58551</v>
+        <v>-34.622044</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -4627,7 +4533,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>AGU-L</t>
+          <t>PCH-M</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -4639,17 +4545,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -4659,7 +4565,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -4674,7 +4580,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -4687,7 +4593,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -4696,10 +4602,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.435017</v>
+        <v>-58.443232</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.622044</v>
+        <v>-34.620007</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -4713,96 +4619,10 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PCH-M</t>
+          <t>PCH-G</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>4698</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>8/29/2025</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>ICD30593982</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M18" t="n">
-        <v>-58.443232</v>
-      </c>
-      <c r="N18" t="n">
-        <v>-34.620007</v>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>PCH-G</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>